<commit_message>
CSV fileS of SOME dataAAAAAAAAAAAAAAAAAAA
kol project we ento tybeen :"
</commit_message>
<xml_diff>
--- a/csv files/series.xlsx
+++ b/csv files/series.xlsx
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,7 +1462,7 @@
         <v>123123123</v>
       </c>
       <c r="H9">
-        <v>789789789</v>
+        <v>78974589789</v>
       </c>
       <c r="I9" t="s">
         <v>69</v>
@@ -1538,7 +1538,7 @@
         <v>3123123</v>
       </c>
       <c r="H11">
-        <v>78978978</v>
+        <v>43534545345345</v>
       </c>
       <c r="I11" t="s">
         <v>73</v>
@@ -1576,7 +1576,7 @@
         <v>123123123</v>
       </c>
       <c r="H12">
-        <v>978978978</v>
+        <v>3454545345345</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>75</v>
@@ -1652,7 +1652,7 @@
         <v>123123</v>
       </c>
       <c r="H14">
-        <v>78978978978</v>
+        <v>345345454534534</v>
       </c>
       <c r="I14" t="s">
         <v>79</v>
@@ -1690,7 +1690,7 @@
         <v>23445432</v>
       </c>
       <c r="H15">
-        <v>9789789789</v>
+        <v>45345345345345</v>
       </c>
       <c r="I15" t="s">
         <v>81</v>
@@ -1728,7 +1728,7 @@
         <v>53453</v>
       </c>
       <c r="H16">
-        <v>789789789</v>
+        <v>343453454534545</v>
       </c>
       <c r="I16" t="s">
         <v>83</v>
@@ -1804,7 +1804,7 @@
         <v>345345</v>
       </c>
       <c r="H18">
-        <v>789789789</v>
+        <v>34545345345454</v>
       </c>
       <c r="I18" t="s">
         <v>87</v>
@@ -1842,7 +1842,7 @@
         <v>3454</v>
       </c>
       <c r="H19">
-        <v>87879979</v>
+        <v>3434543345</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>89</v>
@@ -1880,7 +1880,7 @@
         <v>34534</v>
       </c>
       <c r="H20">
-        <v>78978978</v>
+        <v>3.45453453454353E+18</v>
       </c>
       <c r="I20" t="s">
         <v>91</v>

</xml_diff>